<commit_message>
Update fcns and tmplte to plot 1 and 4-panel plots
</commit_message>
<xml_diff>
--- a/H_Index_Rosenheim_Demo.xlsx
+++ b/H_Index_Rosenheim_Demo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beros\Box\UDrive_brosenheim\My_Documents\PyCode\PubPy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC1A5016-7178-4925-87B5-7F868080E74C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E960B58A-35F4-4C94-AD86-F608956B9F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{47CF98EE-F03B-422A-82DC-7319A007806E}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" firstSheet="4" activeTab="12" xr2:uid="{47CF98EE-F03B-422A-82DC-7319A007806E}"/>
   </bookViews>
   <sheets>
     <sheet name="20130301" sheetId="12" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="20200106" sheetId="9" r:id="rId10"/>
     <sheet name="20210128" sheetId="10" r:id="rId11"/>
     <sheet name="20220117" sheetId="11" r:id="rId12"/>
+    <sheet name="20230101" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1236" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="133">
   <si>
     <t>Year</t>
   </si>
@@ -425,6 +426,27 @@
   </si>
   <si>
     <t>Engineered continental-scale rivers can drive changes in the carbon cycle</t>
+  </si>
+  <si>
+    <t>Proceedings of the National Academy of Science</t>
+  </si>
+  <si>
+    <t>Enhanced trace element mobilization by Earth’s ice sheets</t>
+  </si>
+  <si>
+    <t>History of the Larsen C Ice Shelf reconstructed from sub–ice shelf and offshore sediments</t>
+  </si>
+  <si>
+    <t>Quaternary Geochronology</t>
+  </si>
+  <si>
+    <t>New radiocarbon estimation method for carbonate-poor sediments: A case study of ramped pyrolysis 14C dating of postglacial deposits from the Alaskan margin, Arctic Ocean</t>
+  </si>
+  <si>
+    <t>A FRAMEWORK FOR TRANSDISCIPLINARY RADIOCARBON RESEARCH: USE OF NATURAL-LEVEL AND ELEVATED-LEVEL 14C IN ANTARCTIC FIELD RESEARCH</t>
+  </si>
+  <si>
+    <t>Mapping spatial and temporal variation of seafloor organic matter Δ14C and δ13C in the Northern Gulf of Mexico following the Deepwater Horizon Oil Spill</t>
   </si>
 </sst>
 </file>
@@ -781,7 +803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F71C2357-71A2-4AFE-8E02-7BBD3D36C976}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:D19"/>
     </sheetView>
   </sheetViews>
@@ -3021,7 +3043,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A77F924-D204-4732-BF1E-AF93396C5D24}">
   <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView topLeftCell="A66" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:D71"/>
     </sheetView>
   </sheetViews>
@@ -4027,6 +4049,1093 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F74F38F3-5DA9-4E27-86E7-E677358DC002}">
+  <dimension ref="A1:D76"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="17.3984375" customWidth="1"/>
+    <col min="3" max="3" width="27.3984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A2" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="1">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="A3" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="1">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+      <c r="A4" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="1">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+      <c r="A5" s="1">
+        <v>2008</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A6" s="1">
+        <v>2010</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A7" s="1">
+        <v>2018</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="1">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A8" s="1">
+        <v>2011</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="1">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+      <c r="A9" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="1">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A10" s="1">
+        <v>2012</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="1">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A11" s="1">
+        <v>2004</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="1">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A12" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="1">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A13" s="1">
+        <v>2013</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A14" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+      <c r="A15" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+      <c r="A16" s="1">
+        <v>2002</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+      <c r="A17" s="1">
+        <v>2013</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+      <c r="A18" s="1">
+        <v>2005</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A19" s="1">
+        <v>2010</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+      <c r="A20" s="1">
+        <v>2005</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A21" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="114" x14ac:dyDescent="0.45">
+      <c r="A22" s="1">
+        <v>2007</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A23" s="1">
+        <v>2018</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A24" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A25" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+      <c r="A26" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A27" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A28" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D28" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+      <c r="A29" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D29" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+      <c r="A30" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D30" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+      <c r="A31" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D31" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A32" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D32" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A33" s="1">
+        <v>2013</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D33" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A34" s="1">
+        <v>2018</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D34" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+      <c r="A35" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D35" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A36" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D36" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="114" x14ac:dyDescent="0.45">
+      <c r="A37" s="1">
+        <v>2013</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D37" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+      <c r="A38" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D38" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+      <c r="A39" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D39" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A40" s="1">
+        <v>2006</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D40" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A41" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D41" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A42" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D42" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A43" s="1">
+        <v>2001</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D43" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+      <c r="A44" s="1">
+        <v>2009</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D44" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A45" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D45" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+      <c r="A46" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D46" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A47" s="1">
+        <v>2018</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D47" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+      <c r="A48" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D48" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+      <c r="A49" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D49" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+      <c r="A50" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D50" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="114" x14ac:dyDescent="0.45">
+      <c r="A51" s="1">
+        <v>2008</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D51" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A52" s="1">
+        <v>2018</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D52" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+      <c r="A53" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D53" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+      <c r="A54" s="1">
+        <v>2018</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D54" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+      <c r="A55" s="1">
+        <v>2008</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D55" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A56" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D56" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A57" s="1">
+        <v>2013</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D57" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A58" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D58" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A59" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D59" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+      <c r="A60" s="1">
+        <v>2007</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D60" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="114" x14ac:dyDescent="0.45">
+      <c r="A61" s="1">
+        <v>2007</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D61" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A62" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D62" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+      <c r="A63" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D63" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A64" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D64" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A65" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D65" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A66" s="1">
+        <v>2018</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D66" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A67" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D67" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+      <c r="A68" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D68" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A69" s="1">
+        <v>2012</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D69" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+      <c r="A70" s="1">
+        <v>2005</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D70" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+      <c r="A71" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D71" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+      <c r="A72" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D72" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A73" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D73" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A74" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D74" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A75" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D75" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A76" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D76" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D76">
+    <sortCondition descending="1" ref="D2:D76"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>